<commit_message>
Updated Issue documentation. Improved SearchField
</commit_message>
<xml_diff>
--- a/Blazor.Tools/Data/SetTargetTable - PettyCash sample data.xlsx
+++ b/Blazor.Tools/Data/SetTargetTable - PettyCash sample data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\Blazor.Tools\Blazor.Tools\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0767e6b8eac1c558/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC60F2-274D-4D81-BCE5-8B59123DD05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{170618D1-CAE1-4E4A-A82C-31C8E1064FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48E023C5-D0CE-4762-AB2F-5FB32916CFC2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BB3A784-C868-4B78-84AB-1178D37F3375}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="94">
   <si>
     <t>PettyCash</t>
   </si>
@@ -300,6 +300,47 @@
   </si>
   <si>
     <t>Lookup Condition</t>
+  </si>
+  <si>
+    <t>Example: Source Field = F5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  1.1. Add a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LookupFieldConditionEnum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that would take care of this case scenario. It should initially contain these properties:</t>
+    </r>
+  </si>
+  <si>
+    <t>Note: The Split refers to the element on the array split from the original string value e.g.: "John Vic".</t>
+  </si>
+  <si>
+    <t>The string is delimeted by a space (" ") character.</t>
+  </si>
+  <si>
+    <t>The Value property refers to the actual field value "John Vic".</t>
+  </si>
+  <si>
+    <t>A more appropriate example for the Value property usage is SourceField=F7.</t>
   </si>
 </sst>
 </file>
@@ -1002,17 +1043,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13ABE66D-F1A4-4071-84EC-B26B8CD5BABA}">
-  <dimension ref="B2:O62"/>
+  <dimension ref="B2:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G54" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" customWidth="1"/>
@@ -1070,7 +1112,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1150,7 @@
       <c r="N4" s="14"/>
       <c r="O4" s="16"/>
     </row>
-    <row r="5" spans="2:15" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
       <c r="D5" s="26" t="s">
@@ -1206,7 +1248,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="2:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1838,6 +1880,137 @@
         <v>86</v>
       </c>
     </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67" t="s">
+        <v>73</v>
+      </c>
+      <c r="G67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>68</v>
+      </c>
+      <c r="F68" t="s">
+        <v>74</v>
+      </c>
+      <c r="G68" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>69</v>
+      </c>
+      <c r="F69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>71</v>
+      </c>
+      <c r="E84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F84" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>